<commit_message>
Some Hybrid and ItemfSLIM outputs. Item SCM and UserSLIM
</commit_message>
<xml_diff>
--- a/Grade.xlsx
+++ b/Grade.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,21 +524,35 @@
       <c r="A4" s="2">
         <v>42705</v>
       </c>
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4">
+        <f>(8.67+8.21)/2</f>
+        <v>8.4400000000000013</v>
+      </c>
+      <c r="D4">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>7.5</v>
+      </c>
       <c r="F4">
         <f>AVERAGE($C$2:C4)</f>
-        <v>7.3049999999999997</v>
+        <v>7.6833333333333336</v>
       </c>
       <c r="G4">
         <f>SUM($D$3:D4)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <f>SUM($E$2:E4)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>MROUND(SUM(F4:H4),1)</f>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -547,19 +561,19 @@
       </c>
       <c r="F5">
         <f>AVERAGE($C$2:C5)</f>
-        <v>7.3049999999999997</v>
+        <v>7.6833333333333336</v>
       </c>
       <c r="G5">
         <f>SUM($D$3:D5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <f>SUM($E$2:E5)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -568,19 +582,19 @@
       </c>
       <c r="F6">
         <f>AVERAGE($C$2:C6)</f>
-        <v>7.3049999999999997</v>
+        <v>7.6833333333333336</v>
       </c>
       <c r="G6">
         <f>SUM($D$3:D6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f>SUM($E$2:E6)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -589,19 +603,19 @@
       </c>
       <c r="F7">
         <f>AVERAGE($C$2:C7)</f>
-        <v>7.3049999999999997</v>
+        <v>7.6833333333333336</v>
       </c>
       <c r="G7">
         <f>SUM($D$3:D7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <f>SUM($E$2:E7)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Item fSCM; ItemSLIM, SCM and fSLIM with implicit ratings
</commit_message>
<xml_diff>
--- a/Grade.xlsx
+++ b/Grade.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +469,7 @@
         <v>9</v>
       </c>
       <c r="E2">
+        <f>2*1.5</f>
         <v>3</v>
       </c>
       <c r="F2">
@@ -536,7 +537,8 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>7.5</v>
+        <f>4*1.5</f>
+        <v>6</v>
       </c>
       <c r="F4">
         <f>AVERAGE($C$2:C4)</f>
@@ -548,20 +550,33 @@
       </c>
       <c r="H4">
         <f>SUM($E$2:E4)</f>
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="I4">
         <f>MROUND(SUM(F4:H4),1)</f>
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>42719</v>
       </c>
+      <c r="B5">
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <f>(6.7+6.9)/2</f>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <f>AVERAGE($C$2:C5)</f>
-        <v>7.6833333333333336</v>
+        <v>7.4625000000000004</v>
       </c>
       <c r="G5">
         <f>SUM($D$3:D5)</f>
@@ -569,20 +584,34 @@
       </c>
       <c r="H5">
         <f>SUM($E$2:E5)</f>
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>42384</v>
       </c>
+      <c r="B6">
+        <f>40</f>
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <f>6.8</f>
+        <v>6.8</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <f>AVERAGE($C$2:C6)</f>
-        <v>7.6833333333333336</v>
+        <v>7.33</v>
       </c>
       <c r="G6">
         <f>SUM($D$3:D6)</f>
@@ -590,24 +619,39 @@
       </c>
       <c r="H6">
         <f>SUM($E$2:E6)</f>
-        <v>10.5</v>
+        <v>9</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>42401</v>
       </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <f>17-16*LOG((B7-1)/(70-1) + 1,2)</f>
+        <v>8.2050075844219883</v>
+      </c>
+      <c r="D7">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>1.5*1</f>
+        <v>1.5</v>
+      </c>
       <c r="F7">
-        <f>AVERAGE($C$2:C7)</f>
-        <v>7.6833333333333336</v>
+        <f>SUM(C2:C7,C7)/7</f>
+        <v>7.5800021669777111</v>
       </c>
       <c r="G7">
         <f>SUM($D$3:D7)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7">
         <f>SUM($E$2:E7)</f>
@@ -615,7 +659,7 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>